<commit_message>
Change form to be more friendly to international Alumni
</commit_message>
<xml_diff>
--- a/form_submissions.xlsx
+++ b/form_submissions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B3857D-6AA7-964A-96E3-6A1E24D6B00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD0B981-D27B-C440-BD46-35B086329FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>